<commit_message>
Cleaned up the chart and added title. Working on Pie chart.
</commit_message>
<xml_diff>
--- a/lines.xlsx
+++ b/lines.xlsx
@@ -183,6 +183,21 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Counterfeit Crimes by District</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
     <plotArea>
       <barChart>
         <barDir val="col"/>
@@ -192,7 +207,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!A8</f>
+              <f>'Sheet'!A10</f>
             </strRef>
           </tx>
           <spPr>
@@ -200,9 +215,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$8:$M$8</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$A$9:$A$13</f>
+              <f>'Sheet'!$B$10:$M$10</f>
             </numRef>
           </val>
         </ser>
@@ -211,7 +231,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!B8</f>
+              <f>'Sheet'!A11</f>
             </strRef>
           </tx>
           <spPr>
@@ -219,9 +239,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$8:$M$8</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$B$9:$B$13</f>
+              <f>'Sheet'!$B$11:$M$11</f>
             </numRef>
           </val>
         </ser>
@@ -230,7 +255,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'Sheet'!C8</f>
+              <f>'Sheet'!A12</f>
             </strRef>
           </tx>
           <spPr>
@@ -238,9 +263,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$8:$M$8</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$C$9:$C$13</f>
+              <f>'Sheet'!$B$12:$M$12</f>
             </numRef>
           </val>
         </ser>
@@ -249,7 +279,7 @@
           <order val="3"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D8</f>
+              <f>'Sheet'!A13</f>
             </strRef>
           </tx>
           <spPr>
@@ -257,180 +287,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$8:$M$8</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$9:$D$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!E8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$E$9:$E$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!F8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$F$9:$F$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!G8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$G$9:$G$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="7"/>
-          <order val="7"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!H8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$H$9:$H$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="8"/>
-          <order val="8"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!I8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$I$9:$I$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="9"/>
-          <order val="9"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!J8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$J$9:$J$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="10"/>
-          <order val="10"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!K8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$K$9:$K$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="11"/>
-          <order val="11"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!L8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$L$9:$L$13</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="12"/>
-          <order val="12"/>
-          <tx>
-            <strRef>
-              <f>'Sheet'!M8</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet'!$M$9:$M$13</f>
+              <f>'Sheet'!$B$13:$M$13</f>
             </numRef>
           </val>
         </ser>
@@ -479,7 +343,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <ext cx="7308000" cy="1710000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>

</xml_diff>

<commit_message>
Added Pie chart using the same process as Bar Chart.
</commit_message>
<xml_diff>
--- a/lines.xlsx
+++ b/lines.xlsx
@@ -334,6 +334,58 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>% Counterfeit Crimes</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$O$7:$P$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$O$8:$P$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -353,6 +405,28 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>14</col>
+      <colOff>0</colOff>
+      <row>13</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2430000" cy="1710000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>

</xml_diff>